<commit_message>
04/16/2024 new updates and bugs
</commit_message>
<xml_diff>
--- a/wwwroot/Uploads/Excel/234129873 - THIS IS A DESCRIPTION.xlsx
+++ b/wwwroot/Uploads/Excel/234129873 - THIS IS A DESCRIPTION.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kgahete\kgajete\Desktop\BUSINESS CONTROL\SOURCING FORM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E5C1AE-0922-4F91-A648-CDC0F8313EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7CEE67-4113-4064-9037-E583D21B3357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38AD120D-C7C0-421F-989A-B3D76F33A526}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>Product:</t>
   </si>
@@ -205,6 +205,27 @@
   </si>
   <si>
     <t>K.GAJETE</t>
+  </si>
+  <si>
+    <t>STANDOFF F M3 X 69MM</t>
+  </si>
+  <si>
+    <t>ADSDSADAS</t>
+  </si>
+  <si>
+    <t>DDAS</t>
+  </si>
+  <si>
+    <t>1FDSGSDFSF</t>
+  </si>
+  <si>
+    <t>FGWTWERR</t>
+  </si>
+  <si>
+    <t>SFWER</t>
+  </si>
+  <si>
+    <t>234R2WEFD</t>
   </si>
 </sst>
 </file>
@@ -418,7 +439,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -545,6 +566,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1008,9 +1032,9 @@
   </sheetPr>
   <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1290,32 +1314,80 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
+      <c r="A12" s="30">
+        <v>1</v>
+      </c>
+      <c r="B12" s="30">
+        <v>1</v>
+      </c>
+      <c r="C12" s="31">
+        <v>4102256</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="30">
+        <v>1</v>
+      </c>
+      <c r="H12" s="30">
+        <v>2</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="34" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="35"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
+      <c r="A13" s="35">
+        <v>1</v>
+      </c>
+      <c r="B13" s="36">
+        <v>1</v>
+      </c>
+      <c r="C13" s="37">
+        <v>123456</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="30">
+        <v>1</v>
+      </c>
+      <c r="H13" s="30">
+        <v>1</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="43" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="35"/>

</xml_diff>